<commit_message>
Fix broken TestNG tests
</commit_message>
<xml_diff>
--- a/src/test/java/com/UKTalentHubJava/test_data/ValidLoginDetails.xlsx
+++ b/src/test/java/com/UKTalentHubJava/test_data/ValidLoginDetails.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5A72A3-3454-4B02-929D-4BC2BCD4A9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6791ED6A-F2B6-481D-A762-35C8711B434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="345" windowWidth="12645" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Details" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>123123@email.com</t>
+  </si>
+  <si>
+    <t>PasswordPassword!Password!123</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,8 +466,8 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>123123</v>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>